<commit_message>
The result of 1606
</commit_message>
<xml_diff>
--- a/notebooks/Linear_Regression_Results.xlsx
+++ b/notebooks/Linear_Regression_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZhipuCUI\Dropbox\PC\Desktop\MyDoc\Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00889E7F-7F24-4200-90A8-47588885C09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB191CB6-95C2-425C-A433-0B0FD9F7A39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>OP</t>
   </si>
@@ -74,7 +74,28 @@
     <t>rr24 month</t>
   </si>
   <si>
-    <t>s</t>
+    <t>rr24 + DJ_0 Degreed</t>
+  </si>
+  <si>
+    <t>rr24 Month</t>
+  </si>
+  <si>
+    <t>3 4</t>
+  </si>
+  <si>
+    <t>3 2</t>
+  </si>
+  <si>
+    <t>6 10</t>
+  </si>
+  <si>
+    <t>2 4</t>
+  </si>
+  <si>
+    <t>4 3</t>
+  </si>
+  <si>
+    <t>3 1</t>
   </si>
 </sst>
 </file>
@@ -425,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
@@ -549,10 +570,10 @@
       <c r="F4" s="2">
         <v>0.26415660004795199</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="4">
         <v>0.21553333204208899</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="4">
         <v>0.21583597255293399</v>
       </c>
       <c r="I4" s="2">
@@ -590,71 +611,103 @@
       <c r="I5" s="2">
         <v>0.16549722688803001</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="4">
         <v>0.187688414962113</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.224218941512623</v>
+        <v>15</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.22627002314956601</v>
       </c>
       <c r="C6" s="3">
-        <v>0.17684561772530899</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.18374600000455299</v>
+        <v>0.17540495061797601</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.18602474770376101</v>
       </c>
       <c r="E6" s="3">
-        <v>0.19478518594703401</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.25370158150904798</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.225553397465908</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.22589179292412601</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.16530291725530499</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.187953779534586</v>
+        <v>0.193970253076476</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.254960912590179</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.21528576200065999</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.21557448940438201</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.166280355376205</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.18626718982611701</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.224218941512623</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.17684561772530899</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.18374600000455299</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.19478518594703401</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.25370158150904798</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.225553397465908</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.22589179292412601</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.16530291725530499</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.187953779534586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4">
         <v>0.232207165609186</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C8" s="4">
         <v>0.184029934437413</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8" s="4">
         <v>0.22460202427856699</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E8" s="4">
         <v>0.19669659688099</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F8" s="4">
         <v>0.27689647864362898</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G8" s="4">
         <v>0.230652070071515</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H8" s="4">
         <v>0.230968689491617</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I8" s="4">
         <v>0.21219835783232199</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J8" s="4">
         <v>0.18486863862670999</v>
       </c>
     </row>
@@ -666,15 +719,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60A1903-4C81-4DBE-A021-69A1F350D10C}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -790,10 +843,10 @@
       <c r="F4" s="2">
         <v>9</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="4">
         <v>7</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="4">
         <v>7</v>
       </c>
       <c r="I4" s="2">
@@ -831,71 +884,103 @@
       <c r="I5" s="2">
         <v>3</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3">
-        <v>3</v>
-      </c>
-      <c r="D6" s="3">
-        <v>3</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2">
-        <v>2</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3">
-        <v>4</v>
-      </c>
-      <c r="J6" s="2">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4">
         <v>4</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="4">
         <v>4</v>
       </c>
-      <c r="E7" s="2">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>3</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3</v>
+      </c>
+      <c r="G8" s="4">
         <v>1</v>
       </c>
-      <c r="H7" s="2">
-        <v>2</v>
-      </c>
-      <c r="I7" s="2">
-        <v>3</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="H8" s="4">
+        <v>2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>3</v>
+      </c>
+      <c r="J8" s="4">
         <v>2</v>
       </c>
     </row>
@@ -907,7 +992,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D140CDE-778D-4B68-9B02-67839FD39725}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
@@ -980,11 +1065,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F7" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
The end of week2.
This contains multitype of LR. More detailed work coming at week 3.
</commit_message>
<xml_diff>
--- a/notebooks/Linear_Regression_Results.xlsx
+++ b/notebooks/Linear_Regression_Results.xlsx
@@ -8,26 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZhipuCUI\Dropbox\PC\Desktop\MyDoc\Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB191CB6-95C2-425C-A433-0B0FD9F7A39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EF9489-CDC0-4980-8419-2CAA74FA5450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rRMSE" sheetId="1" r:id="rId1"/>
     <sheet name="Degree" sheetId="2" r:id="rId2"/>
     <sheet name=" Month" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>OP</t>
   </si>
@@ -71,31 +81,49 @@
     <t>rr24 + DJ_6</t>
   </si>
   <si>
-    <t>rr24 month</t>
-  </si>
-  <si>
     <t>rr24 + DJ_0 Degreed</t>
   </si>
   <si>
-    <t>rr24 Month</t>
-  </si>
-  <si>
     <t>3 4</t>
   </si>
   <si>
     <t>3 2</t>
   </si>
   <si>
-    <t>6 10</t>
-  </si>
-  <si>
-    <t>2 4</t>
-  </si>
-  <si>
     <t>4 3</t>
   </si>
   <si>
     <t>3 1</t>
+  </si>
+  <si>
+    <t>rr24 Best Month</t>
+  </si>
+  <si>
+    <t>rr24 + DJ_6 Degreed</t>
+  </si>
+  <si>
+    <t>DJ_0 Best Month</t>
+  </si>
+  <si>
+    <t>DJ_6 Best Month</t>
+  </si>
+  <si>
+    <t>4 1</t>
+  </si>
+  <si>
+    <t>4 2</t>
+  </si>
+  <si>
+    <t>2 7</t>
+  </si>
+  <si>
+    <t>2 8</t>
+  </si>
+  <si>
+    <t>5 3</t>
+  </si>
+  <si>
+    <t>Min</t>
   </si>
 </sst>
 </file>
@@ -117,7 +145,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,12 +155,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,9 +180,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -446,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,19 +511,19 @@
         <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>0.248933637506596</v>
+        <v>0.25030009604009001</v>
       </c>
       <c r="C2" s="2">
-        <v>0.21166547484477799</v>
+        <v>0.21210011646907101</v>
       </c>
       <c r="D2" s="2">
-        <v>0.24892582175024</v>
+        <v>0.24841759512542499</v>
       </c>
       <c r="E2" s="2">
         <v>0.22547719969041999</v>
       </c>
       <c r="F2" s="2">
-        <v>0.29244879068383201</v>
+        <v>0.29052001638368602</v>
       </c>
       <c r="G2" s="2">
         <v>0.232676106954472</v>
@@ -513,7 +532,7 @@
         <v>0.232676106954472</v>
       </c>
       <c r="I2" s="2">
-        <v>0.22737902143136801</v>
+        <v>0.227455442185684</v>
       </c>
       <c r="J2" s="2">
         <v>0.20852417057938499</v>
@@ -524,31 +543,31 @@
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>0.231413956924507</v>
+        <v>0.23131246555940099</v>
       </c>
       <c r="C3" s="2">
-        <v>0.18261486055179199</v>
+        <v>0.18245808061036001</v>
       </c>
       <c r="D3" s="2">
-        <v>0.198993422752821</v>
+        <v>0.19787959249279599</v>
       </c>
       <c r="E3" s="2">
-        <v>0.201367642478398</v>
+        <v>0.200452752798189</v>
       </c>
       <c r="F3" s="2">
-        <v>0.26602750726437802</v>
+        <v>0.265062213022835</v>
       </c>
       <c r="G3" s="2">
-        <v>0.21685011930178699</v>
+        <v>0.21668737189297799</v>
       </c>
       <c r="H3" s="2">
-        <v>0.21710364695273399</v>
+        <v>0.21612725428521101</v>
       </c>
       <c r="I3" s="2">
-        <v>0.176838551098321</v>
+        <v>0.17594996334332499</v>
       </c>
       <c r="J3" s="2">
-        <v>0.190641145868576</v>
+        <v>0.19002626324910801</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -556,31 +575,31 @@
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>0.23058194205235</v>
+        <v>0.230229031872421</v>
       </c>
       <c r="C4" s="2">
-        <v>0.18444190679507699</v>
+        <v>0.184594814094966</v>
       </c>
       <c r="D4" s="2">
-        <v>0.19952794537291799</v>
+        <v>0.198865483318376</v>
       </c>
       <c r="E4" s="2">
-        <v>0.20251128434718901</v>
+        <v>0.202070076104678</v>
       </c>
       <c r="F4" s="2">
-        <v>0.26415660004795199</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.21553333204208899</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.21583597255293399</v>
+        <v>0.26211515781288303</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.21482242323931899</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.21525341082100699</v>
       </c>
       <c r="I4" s="2">
-        <v>0.177945689196644</v>
+        <v>0.177522865572351</v>
       </c>
       <c r="J4" s="2">
-        <v>0.191042587596431</v>
+        <v>0.19198166131575001</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -588,127 +607,264 @@
         <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>0.224760329421137</v>
+        <v>0.224001941418562</v>
       </c>
       <c r="C5" s="2">
-        <v>0.17954049941365799</v>
+        <v>0.178991701273054</v>
       </c>
       <c r="D5" s="2">
-        <v>0.18642733264321801</v>
+        <v>0.185889346868086</v>
       </c>
       <c r="E5" s="2">
-        <v>0.19483209254866299</v>
+        <v>0.19361898742554301</v>
       </c>
       <c r="F5" s="2">
-        <v>0.25435264652610801</v>
+        <v>0.25394635961244599</v>
       </c>
       <c r="G5" s="2">
-        <v>0.223375938919541</v>
+        <v>0.22256369790945499</v>
       </c>
       <c r="H5" s="2">
-        <v>0.22321385040538999</v>
+        <v>0.22340526213919101</v>
       </c>
       <c r="I5" s="2">
-        <v>0.16549722688803001</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0.187688414962113</v>
+        <v>0.165227363129058</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.186892343109339</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2">
-        <v>0.22627002314956601</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.17540495061797601</v>
+        <v>0.22348821809842001</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.178812519857976</v>
       </c>
       <c r="D6" s="2">
-        <v>0.18602474770376101</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.193970253076476</v>
+        <v>0.18310018729048999</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.19484540551682999</v>
       </c>
       <c r="F6" s="2">
-        <v>0.254960912590179</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.21528576200065999</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.21557448940438201</v>
+        <v>0.25150722534741898</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.225970026007488</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.226475481650316</v>
       </c>
       <c r="I6" s="2">
-        <v>0.166280355376205</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0.18626718982611701</v>
+        <v>0.16576681297100901</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.18872411611031001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.224218941512623</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.17684561772530899</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.18374600000455299</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.19478518594703401</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.25370158150904798</v>
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.225474205545939</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.17578495614477599</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.187631850262652</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.19390791755679601</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.25573709325066801</v>
       </c>
       <c r="G7" s="2">
-        <v>0.225553397465908</v>
+        <v>0.21575690698784999</v>
       </c>
       <c r="H7" s="2">
-        <v>0.22589179292412601</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.16530291725530499</v>
+        <v>0.215987861164541</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.16641979431051701</v>
       </c>
       <c r="J7" s="2">
-        <v>0.187953779534586</v>
+        <v>0.186382991634749</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0.232207165609186</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.184029934437413</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.22460202427856699</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.19669659688099</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.27689647864362898</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.230652070071515</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0.230968689491617</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0.21219835783232199</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0.18486863862670999</v>
+        <v>20</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.223181476178473</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.17454503413035599</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.18379178287037601</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.192653433263517</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.252097403994825</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.21519061768822201</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.21391699032956499</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.164844290925793</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.18746966576718699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.231396088067195</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.18423721331885501</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.22529794362123101</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.19617962606261699</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.278385966772704</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.230635912945057</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.23078158008496499</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.211853685858402</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.18530569062497501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.221087461875908</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.168917083150051</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.182923077146665</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.184540978634334</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.24890819877874201</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.21839211850056001</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.21734794447488301</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.16725372010780701</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.20025152714434399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.21837576980780199</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.168829024626899</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.179688049306265</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.18426404385608899</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.246391957843791</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.21791908605926999</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.217789180940273</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.16406203051752</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.198335072258704</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2">
+        <f>MIN(B2:B11)</f>
+        <v>0.21837576980780199</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ref="C12:J12" si="0">MIN(C2:C11)</f>
+        <v>0.168829024626899</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.179688049306265</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18426404385608899</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.246391957843791</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21482242323931899</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21391699032956499</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16406203051752</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18530569062497501</v>
       </c>
     </row>
   </sheetData>
@@ -719,15 +875,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60A1903-4C81-4DBE-A021-69A1F350D10C}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -771,7 +927,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -797,7 +953,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2">
         <v>7</v>
@@ -806,22 +962,22 @@
         <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2">
         <v>10</v>
       </c>
       <c r="I3" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -829,24 +985,24 @@
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F4" s="2">
         <v>9</v>
       </c>
-      <c r="G4" s="4">
-        <v>7</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="G4" s="3">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2">
         <v>7</v>
       </c>
       <c r="I4" s="2">
@@ -884,105 +1040,216 @@
       <c r="I5" s="2">
         <v>3</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3</v>
-      </c>
-      <c r="E7" s="4">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3">
-        <v>4</v>
-      </c>
-      <c r="J7" s="2">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4">
-        <v>3</v>
-      </c>
-      <c r="C8" s="4">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
         <v>4</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="2">
         <v>4</v>
       </c>
-      <c r="E8" s="4">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4">
-        <v>3</v>
-      </c>
-      <c r="G8" s="4">
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2">
         <v>1</v>
       </c>
-      <c r="H8" s="4">
-        <v>2</v>
-      </c>
-      <c r="I8" s="4">
-        <v>3</v>
-      </c>
-      <c r="J8" s="4">
-        <v>2</v>
-      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4</v>
+      </c>
+      <c r="G10" s="2">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2">
+        <v>9</v>
+      </c>
+      <c r="I10" s="2">
+        <v>9</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3">
+        <v>3</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -992,15 +1259,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D140CDE-778D-4B68-9B02-67839FD39725}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="14.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1034,38 +1302,103 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4">
         <v>12</v>
       </c>
-      <c r="C2" s="5">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="C2" s="4">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
         <v>6</v>
       </c>
-      <c r="F2" s="5">
-        <v>3</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="F2" s="4">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4">
         <v>10</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>10</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>12</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4">
+        <v>9</v>
+      </c>
+      <c r="J3" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4">
+        <v>9</v>
+      </c>
+      <c r="I4" s="4">
+        <v>9</v>
+      </c>
+      <c r="J4" s="4">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>